<commit_message>
Added a stop at the end for CTRL+Down
</commit_message>
<xml_diff>
--- a/basic-arithmetic-number-sense/Card Types/{Data Sheet Chunk} 1. Addition and Subtraction.xlsx
+++ b/basic-arithmetic-number-sense/Card Types/{Data Sheet Chunk} 1. Addition and Subtraction.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>Operation</t>
   </si>
@@ -105,9 +105,6 @@
   <si>
     <t>sub</t>
   </si>
-  <si>
-    <t>arith_sub_g01_00_o01_02</t>
-  </si>
 </sst>
 </file>
 
@@ -151,12 +148,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF0070C0"/>
@@ -193,8 +185,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
     <tableStyle name="Table Style 1" pivot="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="4"/>
-      <tableStyleElement type="headerRow" dxfId="3"/>
+      <tableStyleElement type="wholeTable" dxfId="3"/>
+      <tableStyleElement type="headerRow" dxfId="2"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -9144,7 +9136,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" t="str">
         <f>IF(ISNUMBER(C209),"arith_" &amp; INDEX(Operations[],J209,2) &amp; "_g" &amp; TEXT(C209, "00") &amp; "_" &amp; TEXT(D209, "00") &amp; "_o" &amp; TEXT(E209, "00") &amp; IF(AND(ISNUMBER(F209), F209&lt;&gt;E209), "_" &amp; TEXT(F209, "00"), ""), "")</f>
         <v>arith_sub_g09_00_o09_10</v>
@@ -9186,7 +9178,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" t="str">
         <f>IF(ISNUMBER(C210),"arith_" &amp; INDEX(Operations[],J210,2) &amp; "_g" &amp; TEXT(C210, "00") &amp; "_" &amp; TEXT(D210, "00") &amp; "_o" &amp; TEXT(E210, "00") &amp; IF(AND(ISNUMBER(F210), F210&lt;&gt;E210), "_" &amp; TEXT(F210, "00"), ""), "")</f>
         <v>arith_sub_g09_00_o10</v>
@@ -9228,7 +9220,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" t="str">
         <f>IF(ISNUMBER(C211),"arith_" &amp; INDEX(Operations[],J211,2) &amp; "_g" &amp; TEXT(C211, "00") &amp; "_" &amp; TEXT(D211, "00") &amp; "_o" &amp; TEXT(E211, "00") &amp; IF(AND(ISNUMBER(F211), F211&lt;&gt;E211), "_" &amp; TEXT(F211, "00"), ""), "")</f>
         <v/>
@@ -9270,7 +9262,7 @@
         <v/>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" t="str">
         <f>IF(ISNUMBER(C212),"arith_" &amp; INDEX(Operations[],J212,2) &amp; "_g" &amp; TEXT(C212, "00") &amp; "_" &amp; TEXT(D212, "00") &amp; "_o" &amp; TEXT(E212, "00") &amp; IF(AND(ISNUMBER(F212), F212&lt;&gt;E212), "_" &amp; TEXT(F212, "00"), ""), "")</f>
         <v>arith_sub_g10_00_o01_02</v>
@@ -9312,7 +9304,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" t="str">
         <f>IF(ISNUMBER(C213),"arith_" &amp; INDEX(Operations[],J213,2) &amp; "_g" &amp; TEXT(C213, "00") &amp; "_" &amp; TEXT(D213, "00") &amp; "_o" &amp; TEXT(E213, "00") &amp; IF(AND(ISNUMBER(F213), F213&lt;&gt;E213), "_" &amp; TEXT(F213, "00"), ""), "")</f>
         <v>arith_sub_g10_00_o02_03</v>
@@ -9354,7 +9346,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" t="str">
         <f>IF(ISNUMBER(C214),"arith_" &amp; INDEX(Operations[],J214,2) &amp; "_g" &amp; TEXT(C214, "00") &amp; "_" &amp; TEXT(D214, "00") &amp; "_o" &amp; TEXT(E214, "00") &amp; IF(AND(ISNUMBER(F214), F214&lt;&gt;E214), "_" &amp; TEXT(F214, "00"), ""), "")</f>
         <v>arith_sub_g10_00_o03_04</v>
@@ -9396,7 +9388,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" t="str">
         <f>IF(ISNUMBER(C215),"arith_" &amp; INDEX(Operations[],J215,2) &amp; "_g" &amp; TEXT(C215, "00") &amp; "_" &amp; TEXT(D215, "00") &amp; "_o" &amp; TEXT(E215, "00") &amp; IF(AND(ISNUMBER(F215), F215&lt;&gt;E215), "_" &amp; TEXT(F215, "00"), ""), "")</f>
         <v>arith_sub_g10_00_o04_05</v>
@@ -9438,7 +9430,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" t="str">
         <f>IF(ISNUMBER(C216),"arith_" &amp; INDEX(Operations[],J216,2) &amp; "_g" &amp; TEXT(C216, "00") &amp; "_" &amp; TEXT(D216, "00") &amp; "_o" &amp; TEXT(E216, "00") &amp; IF(AND(ISNUMBER(F216), F216&lt;&gt;E216), "_" &amp; TEXT(F216, "00"), ""), "")</f>
         <v>arith_sub_g10_00_o05_06</v>
@@ -9480,7 +9472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" t="str">
         <f>IF(ISNUMBER(C217),"arith_" &amp; INDEX(Operations[],J217,2) &amp; "_g" &amp; TEXT(C217, "00") &amp; "_" &amp; TEXT(D217, "00") &amp; "_o" &amp; TEXT(E217, "00") &amp; IF(AND(ISNUMBER(F217), F217&lt;&gt;E217), "_" &amp; TEXT(F217, "00"), ""), "")</f>
         <v>arith_sub_g10_00_o06_07</v>
@@ -9522,7 +9514,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" t="str">
         <f>IF(ISNUMBER(C218),"arith_" &amp; INDEX(Operations[],J218,2) &amp; "_g" &amp; TEXT(C218, "00") &amp; "_" &amp; TEXT(D218, "00") &amp; "_o" &amp; TEXT(E218, "00") &amp; IF(AND(ISNUMBER(F218), F218&lt;&gt;E218), "_" &amp; TEXT(F218, "00"), ""), "")</f>
         <v>arith_sub_g10_00_o07_08</v>
@@ -9564,7 +9556,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" t="str">
         <f>IF(ISNUMBER(C219),"arith_" &amp; INDEX(Operations[],J219,2) &amp; "_g" &amp; TEXT(C219, "00") &amp; "_" &amp; TEXT(D219, "00") &amp; "_o" &amp; TEXT(E219, "00") &amp; IF(AND(ISNUMBER(F219), F219&lt;&gt;E219), "_" &amp; TEXT(F219, "00"), ""), "")</f>
         <v>arith_sub_g10_00_o08_09</v>
@@ -9606,7 +9598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" t="str">
         <f>IF(ISNUMBER(C220),"arith_" &amp; INDEX(Operations[],J220,2) &amp; "_g" &amp; TEXT(C220, "00") &amp; "_" &amp; TEXT(D220, "00") &amp; "_o" &amp; TEXT(E220, "00") &amp; IF(AND(ISNUMBER(F220), F220&lt;&gt;E220), "_" &amp; TEXT(F220, "00"), ""), "")</f>
         <v>arith_sub_g10_00_o09_10</v>
@@ -9648,7 +9640,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" t="str">
         <f>IF(ISNUMBER(C221),"arith_" &amp; INDEX(Operations[],J221,2) &amp; "_g" &amp; TEXT(C221, "00") &amp; "_" &amp; TEXT(D221, "00") &amp; "_o" &amp; TEXT(E221, "00") &amp; IF(AND(ISNUMBER(F221), F221&lt;&gt;E221), "_" &amp; TEXT(F221, "00"), ""), "")</f>
         <v>arith_sub_g10_00_o10</v>
@@ -9690,7 +9682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" t="str">
         <f>IF(ISNUMBER(C222),"arith_" &amp; INDEX(Operations[],J222,2) &amp; "_g" &amp; TEXT(C222, "00") &amp; "_" &amp; TEXT(D222, "00") &amp; "_o" &amp; TEXT(E222, "00") &amp; IF(AND(ISNUMBER(F222), F222&lt;&gt;E222), "_" &amp; TEXT(F222, "00"), ""), "")</f>
         <v/>
@@ -9731,10 +9723,13 @@
         <f t="shared" si="182"/>
         <v/>
       </c>
+      <c r="K222" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>